<commit_message>
update tx offsets - bct
</commit_message>
<xml_diff>
--- a/tools/data/Tx Offset Calibration.xlsx
+++ b/tools/data/Tx Offset Calibration.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\peter\Documents\MIT\01 STAR Lab\CLICK\Operations\CLICK-A-GSE\tools\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27202863-3965-48DB-A3A7-FBA5D430A5C4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C24460EA-3213-4563-B744-5D4EA5355447}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12450" windowHeight="2508" xr2:uid="{DAC41BD3-2B72-48D2-A016-26083C736758}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Time</t>
   </si>
@@ -64,6 +64,15 @@
   </si>
   <si>
     <t>Bcn y (pxls)</t>
+  </si>
+  <si>
+    <t>OLD</t>
+  </si>
+  <si>
+    <t>Fix calibration</t>
+  </si>
+  <si>
+    <t>BCT Testing</t>
   </si>
 </sst>
 </file>
@@ -105,7 +114,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -119,6 +128,9 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -319,7 +331,7 @@
                   <c:v>34.78</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>36.770000000000003</c:v>
+                  <c:v>36.493385950724246</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>38.4</c:v>
@@ -355,70 +367,70 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="22"/>
                 <c:pt idx="0">
-                  <c:v>-16</c:v>
+                  <c:v>-23</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-16</c:v>
+                  <c:v>-23</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-15</c:v>
+                  <c:v>-22</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-15</c:v>
+                  <c:v>-22</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-15</c:v>
+                  <c:v>-22</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-14</c:v>
+                  <c:v>-21</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-13</c:v>
+                  <c:v>-20</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-13</c:v>
+                  <c:v>-20</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-13</c:v>
+                  <c:v>-20</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-12</c:v>
+                  <c:v>-19</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-12</c:v>
+                  <c:v>-19</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-12</c:v>
+                  <c:v>-19</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-11</c:v>
+                  <c:v>-18</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>-11</c:v>
+                  <c:v>-18</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-11</c:v>
+                  <c:v>-18</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>-24</c:v>
+                  <c:v>-31</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>-24</c:v>
+                  <c:v>-31</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>-23</c:v>
+                  <c:v>-30</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>-22</c:v>
+                  <c:v>-29</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>-21</c:v>
+                  <c:v>-28</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>-13</c:v>
+                  <c:v>-20</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>-25</c:v>
+                  <c:v>-32</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -800,7 +812,7 @@
                   <c:v>34.78</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>36.770000000000003</c:v>
+                  <c:v>36.493385950724246</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>38.4</c:v>
@@ -836,70 +848,70 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="22"/>
                 <c:pt idx="0">
-                  <c:v>194</c:v>
+                  <c:v>121</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>193</c:v>
+                  <c:v>120</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>193</c:v>
+                  <c:v>120</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>193</c:v>
+                  <c:v>120</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>193</c:v>
+                  <c:v>120</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>193</c:v>
+                  <c:v>120</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>193</c:v>
+                  <c:v>120</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>193</c:v>
+                  <c:v>120</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>193</c:v>
+                  <c:v>120</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>193</c:v>
+                  <c:v>120</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>194</c:v>
+                  <c:v>121</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>194</c:v>
+                  <c:v>121</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>195</c:v>
+                  <c:v>122</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>195</c:v>
+                  <c:v>122</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>195</c:v>
+                  <c:v>122</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>195</c:v>
+                  <c:v>122</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>195</c:v>
+                  <c:v>122</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>195</c:v>
+                  <c:v>122</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>195</c:v>
+                  <c:v>122</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>195</c:v>
+                  <c:v>122</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>196</c:v>
+                  <c:v>123</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>197</c:v>
+                  <c:v>124</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2584,10 +2596,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D1705FB-D2BC-4951-B58B-BECDFFB84417}">
-  <dimension ref="A1:S23"/>
+  <dimension ref="A1:T25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2608,7 +2620,7 @@
     <col min="18" max="19" width="8.89453125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:20" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -2648,8 +2660,11 @@
       <c r="M1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="R1" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="4">
         <v>44244</v>
       </c>
@@ -2660,10 +2675,12 @@
         <v>9.9700000000000006</v>
       </c>
       <c r="D2" s="3">
-        <v>-16</v>
+        <f>S2+$D$25</f>
+        <v>-23</v>
       </c>
       <c r="E2" s="3">
-        <v>194</v>
+        <f>T2+$E$25</f>
+        <v>121</v>
       </c>
       <c r="F2" s="1">
         <v>19.62</v>
@@ -2689,8 +2706,17 @@
       <c r="M2" s="1">
         <v>7.9489999999999998</v>
       </c>
+      <c r="R2" s="3">
+        <v>9.9700000000000006</v>
+      </c>
+      <c r="S2" s="3">
+        <v>-16</v>
+      </c>
+      <c r="T2" s="3">
+        <v>194</v>
+      </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="4">
         <v>44244</v>
       </c>
@@ -2701,10 +2727,12 @@
         <v>10.85</v>
       </c>
       <c r="D3" s="3">
-        <v>-16</v>
+        <f t="shared" ref="D3:D23" si="0">S3+$D$25</f>
+        <v>-23</v>
       </c>
       <c r="E3" s="3">
-        <v>193</v>
+        <f t="shared" ref="E3:E23" si="1">T3+$E$25</f>
+        <v>120</v>
       </c>
       <c r="F3" s="1">
         <v>18.89</v>
@@ -2730,8 +2758,17 @@
       <c r="M3" s="1">
         <v>8.85</v>
       </c>
+      <c r="R3" s="3">
+        <v>10.85</v>
+      </c>
+      <c r="S3" s="3">
+        <v>-16</v>
+      </c>
+      <c r="T3" s="3">
+        <v>193</v>
+      </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="4">
         <v>44244</v>
       </c>
@@ -2742,10 +2779,12 @@
         <v>13.36</v>
       </c>
       <c r="D4" s="3">
-        <v>-15</v>
+        <f t="shared" si="0"/>
+        <v>-22</v>
       </c>
       <c r="E4" s="3">
-        <v>193</v>
+        <f t="shared" si="1"/>
+        <v>120</v>
       </c>
       <c r="F4" s="1">
         <v>18.850000000000001</v>
@@ -2771,8 +2810,17 @@
       <c r="M4" s="1">
         <v>11.57</v>
       </c>
+      <c r="R4" s="3">
+        <v>13.36</v>
+      </c>
+      <c r="S4" s="3">
+        <v>-15</v>
+      </c>
+      <c r="T4" s="3">
+        <v>193</v>
+      </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="4">
         <v>44244</v>
       </c>
@@ -2783,10 +2831,12 @@
         <v>14.99</v>
       </c>
       <c r="D5" s="3">
-        <v>-15</v>
+        <f t="shared" si="0"/>
+        <v>-22</v>
       </c>
       <c r="E5" s="3">
-        <v>193</v>
+        <f t="shared" si="1"/>
+        <v>120</v>
       </c>
       <c r="F5" s="1">
         <v>18.78</v>
@@ -2812,8 +2862,17 @@
       <c r="M5" s="1">
         <v>13.31</v>
       </c>
+      <c r="R5" s="3">
+        <v>14.99</v>
+      </c>
+      <c r="S5" s="3">
+        <v>-15</v>
+      </c>
+      <c r="T5" s="3">
+        <v>193</v>
+      </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="4">
         <v>44244</v>
       </c>
@@ -2824,10 +2883,12 @@
         <v>17.440000000000001</v>
       </c>
       <c r="D6" s="3">
-        <v>-15</v>
+        <f t="shared" si="0"/>
+        <v>-22</v>
       </c>
       <c r="E6" s="3">
-        <v>193</v>
+        <f t="shared" si="1"/>
+        <v>120</v>
       </c>
       <c r="F6" s="1">
         <v>19.72</v>
@@ -2853,8 +2914,17 @@
       <c r="M6" s="1">
         <v>15.48</v>
       </c>
+      <c r="R6" s="3">
+        <v>17.440000000000001</v>
+      </c>
+      <c r="S6" s="3">
+        <v>-15</v>
+      </c>
+      <c r="T6" s="3">
+        <v>193</v>
+      </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="4">
         <v>44244</v>
       </c>
@@ -2865,10 +2935,12 @@
         <v>18.600000000000001</v>
       </c>
       <c r="D7" s="3">
-        <v>-14</v>
+        <f t="shared" si="0"/>
+        <v>-21</v>
       </c>
       <c r="E7" s="3">
-        <v>193</v>
+        <f t="shared" si="1"/>
+        <v>120</v>
       </c>
       <c r="F7" s="1">
         <v>18.89</v>
@@ -2894,8 +2966,17 @@
       <c r="M7" s="1">
         <v>17.02</v>
       </c>
+      <c r="R7" s="3">
+        <v>18.600000000000001</v>
+      </c>
+      <c r="S7" s="3">
+        <v>-14</v>
+      </c>
+      <c r="T7" s="3">
+        <v>193</v>
+      </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="4">
         <v>44244</v>
       </c>
@@ -2906,10 +2987,12 @@
         <v>19.71</v>
       </c>
       <c r="D8" s="3">
-        <v>-13</v>
+        <f t="shared" si="0"/>
+        <v>-20</v>
       </c>
       <c r="E8" s="3">
-        <v>193</v>
+        <f t="shared" si="1"/>
+        <v>120</v>
       </c>
       <c r="F8" s="1">
         <v>19.59</v>
@@ -2935,8 +3018,17 @@
       <c r="M8" s="1">
         <v>17.98</v>
       </c>
+      <c r="R8" s="3">
+        <v>19.71</v>
+      </c>
+      <c r="S8" s="3">
+        <v>-13</v>
+      </c>
+      <c r="T8" s="3">
+        <v>193</v>
+      </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="4">
         <v>44244</v>
       </c>
@@ -2947,10 +3039,12 @@
         <v>21.94</v>
       </c>
       <c r="D9" s="3">
-        <v>-13</v>
+        <f t="shared" si="0"/>
+        <v>-20</v>
       </c>
       <c r="E9" s="3">
-        <v>193</v>
+        <f t="shared" si="1"/>
+        <v>120</v>
       </c>
       <c r="F9" s="1">
         <v>17.600000000000001</v>
@@ -2976,8 +3070,17 @@
       <c r="M9" s="1">
         <v>20.03</v>
       </c>
+      <c r="R9" s="3">
+        <v>21.94</v>
+      </c>
+      <c r="S9" s="3">
+        <v>-13</v>
+      </c>
+      <c r="T9" s="3">
+        <v>193</v>
+      </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="4">
         <v>44244</v>
       </c>
@@ -2988,10 +3091,12 @@
         <v>24.28</v>
       </c>
       <c r="D10" s="3">
-        <v>-13</v>
+        <f t="shared" si="0"/>
+        <v>-20</v>
       </c>
       <c r="E10" s="3">
-        <v>193</v>
+        <f t="shared" si="1"/>
+        <v>120</v>
       </c>
       <c r="F10" s="1">
         <v>17.38</v>
@@ -3017,8 +3122,17 @@
       <c r="M10" s="1">
         <v>22.64</v>
       </c>
+      <c r="R10" s="3">
+        <v>24.28</v>
+      </c>
+      <c r="S10" s="3">
+        <v>-13</v>
+      </c>
+      <c r="T10" s="3">
+        <v>193</v>
+      </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="4">
         <v>44244</v>
       </c>
@@ -3029,10 +3143,12 @@
         <v>26.67</v>
       </c>
       <c r="D11" s="3">
-        <v>-12</v>
+        <f t="shared" si="0"/>
+        <v>-19</v>
       </c>
       <c r="E11" s="3">
-        <v>193</v>
+        <f t="shared" si="1"/>
+        <v>120</v>
       </c>
       <c r="F11" s="1">
         <v>19.100000000000001</v>
@@ -3058,8 +3174,17 @@
       <c r="M11" s="1">
         <v>24.97</v>
       </c>
+      <c r="R11" s="3">
+        <v>26.67</v>
+      </c>
+      <c r="S11" s="3">
+        <v>-12</v>
+      </c>
+      <c r="T11" s="3">
+        <v>193</v>
+      </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="4">
         <v>44244</v>
       </c>
@@ -3070,10 +3195,12 @@
         <v>29.92</v>
       </c>
       <c r="D12" s="3">
-        <v>-12</v>
+        <f t="shared" si="0"/>
+        <v>-19</v>
       </c>
       <c r="E12" s="3">
-        <v>194</v>
+        <f t="shared" si="1"/>
+        <v>121</v>
       </c>
       <c r="F12" s="1">
         <v>19.600000000000001</v>
@@ -3099,8 +3226,17 @@
       <c r="M12" s="1">
         <v>28.14</v>
       </c>
+      <c r="R12" s="3">
+        <v>29.92</v>
+      </c>
+      <c r="S12" s="3">
+        <v>-12</v>
+      </c>
+      <c r="T12" s="3">
+        <v>194</v>
+      </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="4">
         <v>44244</v>
       </c>
@@ -3111,10 +3247,12 @@
         <v>33.130000000000003</v>
       </c>
       <c r="D13" s="3">
-        <v>-12</v>
+        <f t="shared" si="0"/>
+        <v>-19</v>
       </c>
       <c r="E13" s="3">
-        <v>194</v>
+        <f t="shared" si="1"/>
+        <v>121</v>
       </c>
       <c r="F13" s="1">
         <v>17.53</v>
@@ -3140,8 +3278,17 @@
       <c r="M13" s="1">
         <v>31.27</v>
       </c>
+      <c r="R13" s="3">
+        <v>33.130000000000003</v>
+      </c>
+      <c r="S13" s="3">
+        <v>-12</v>
+      </c>
+      <c r="T13" s="3">
+        <v>194</v>
+      </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="4">
         <v>44244</v>
       </c>
@@ -3152,10 +3299,12 @@
         <v>34.78</v>
       </c>
       <c r="D14" s="3">
-        <v>-11</v>
+        <f t="shared" si="0"/>
+        <v>-18</v>
       </c>
       <c r="E14" s="3">
-        <v>195</v>
+        <f t="shared" si="1"/>
+        <v>122</v>
       </c>
       <c r="F14" s="1">
         <v>18.649999999999999</v>
@@ -3181,22 +3330,33 @@
       <c r="M14" s="1">
         <v>33.020000000000003</v>
       </c>
+      <c r="R14" s="3">
+        <v>34.78</v>
+      </c>
+      <c r="S14" s="3">
+        <v>-11</v>
+      </c>
+      <c r="T14" s="3">
+        <v>195</v>
+      </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="4">
-        <v>44244</v>
+        <v>44260</v>
       </c>
       <c r="B15" s="2">
-        <v>0.3298611111111111</v>
+        <v>0.5</v>
       </c>
       <c r="C15" s="3">
-        <v>36.770000000000003</v>
+        <v>36.493385950724246</v>
       </c>
       <c r="D15" s="3">
-        <v>-11</v>
+        <f t="shared" si="0"/>
+        <v>-18</v>
       </c>
       <c r="E15" s="3">
-        <v>195</v>
+        <f t="shared" si="1"/>
+        <v>122</v>
       </c>
       <c r="F15" s="1">
         <v>19.18</v>
@@ -3222,8 +3382,23 @@
       <c r="M15" s="1">
         <v>35.1</v>
       </c>
+      <c r="P15" s="4">
+        <v>44244</v>
+      </c>
+      <c r="Q15" s="2">
+        <v>0.3298611111111111</v>
+      </c>
+      <c r="R15" s="3">
+        <v>36.770000000000003</v>
+      </c>
+      <c r="S15" s="3">
+        <v>-11</v>
+      </c>
+      <c r="T15" s="3">
+        <v>195</v>
+      </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="4">
         <v>44244</v>
       </c>
@@ -3234,10 +3409,12 @@
         <v>38.4</v>
       </c>
       <c r="D16" s="3">
-        <v>-11</v>
+        <f t="shared" si="0"/>
+        <v>-18</v>
       </c>
       <c r="E16" s="3">
-        <v>195</v>
+        <f t="shared" si="1"/>
+        <v>122</v>
       </c>
       <c r="F16" s="1">
         <v>19.3</v>
@@ -3263,8 +3440,17 @@
       <c r="M16" s="1">
         <v>36.61</v>
       </c>
+      <c r="R16" s="3">
+        <v>38.4</v>
+      </c>
+      <c r="S16" s="3">
+        <v>-11</v>
+      </c>
+      <c r="T16" s="3">
+        <v>195</v>
+      </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="4">
         <v>44245</v>
       </c>
@@ -3275,10 +3461,12 @@
         <v>1.5</v>
       </c>
       <c r="D17" s="3">
-        <v>-24</v>
+        <f t="shared" si="0"/>
+        <v>-31</v>
       </c>
       <c r="E17" s="3">
-        <v>195</v>
+        <f t="shared" si="1"/>
+        <v>122</v>
       </c>
       <c r="F17" s="1">
         <v>20.65</v>
@@ -3292,8 +3480,17 @@
       <c r="I17" s="1">
         <v>20.89</v>
       </c>
+      <c r="R17" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="S17" s="3">
+        <v>-24</v>
+      </c>
+      <c r="T17" s="3">
+        <v>195</v>
+      </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="4">
         <v>44245</v>
       </c>
@@ -3304,10 +3501,12 @@
         <v>3.16</v>
       </c>
       <c r="D18" s="3">
-        <v>-24</v>
+        <f t="shared" si="0"/>
+        <v>-31</v>
       </c>
       <c r="E18" s="3">
-        <v>195</v>
+        <f t="shared" si="1"/>
+        <v>122</v>
       </c>
       <c r="F18" s="1">
         <v>19.12</v>
@@ -3321,8 +3520,17 @@
       <c r="I18" s="1">
         <v>20.86</v>
       </c>
+      <c r="R18" s="3">
+        <v>3.16</v>
+      </c>
+      <c r="S18" s="3">
+        <v>-24</v>
+      </c>
+      <c r="T18" s="3">
+        <v>195</v>
+      </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="4">
         <v>44245</v>
       </c>
@@ -3333,10 +3541,12 @@
         <v>4.75</v>
       </c>
       <c r="D19" s="3">
-        <v>-23</v>
+        <f t="shared" si="0"/>
+        <v>-30</v>
       </c>
       <c r="E19" s="3">
-        <v>195</v>
+        <f t="shared" si="1"/>
+        <v>122</v>
       </c>
       <c r="F19" s="1">
         <v>19.3</v>
@@ -3350,8 +3560,17 @@
       <c r="I19" s="1">
         <v>19.79</v>
       </c>
+      <c r="R19" s="3">
+        <v>4.75</v>
+      </c>
+      <c r="S19" s="3">
+        <v>-23</v>
+      </c>
+      <c r="T19" s="3">
+        <v>195</v>
+      </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="4">
         <v>44245</v>
       </c>
@@ -3362,10 +3581,12 @@
         <v>6.44</v>
       </c>
       <c r="D20" s="3">
-        <v>-22</v>
+        <f t="shared" si="0"/>
+        <v>-29</v>
       </c>
       <c r="E20" s="3">
-        <v>195</v>
+        <f t="shared" si="1"/>
+        <v>122</v>
       </c>
       <c r="F20" s="1">
         <v>19.27</v>
@@ -3379,8 +3600,17 @@
       <c r="I20" s="1">
         <v>19.8</v>
       </c>
+      <c r="R20" s="3">
+        <v>6.44</v>
+      </c>
+      <c r="S20" s="3">
+        <v>-22</v>
+      </c>
+      <c r="T20" s="3">
+        <v>195</v>
+      </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="4">
         <v>44245</v>
       </c>
@@ -3391,10 +3621,12 @@
         <v>8.4</v>
       </c>
       <c r="D21" s="3">
-        <v>-21</v>
+        <f t="shared" si="0"/>
+        <v>-28</v>
       </c>
       <c r="E21" s="3">
-        <v>195</v>
+        <f t="shared" si="1"/>
+        <v>122</v>
       </c>
       <c r="F21" s="1">
         <v>19.46</v>
@@ -3408,8 +3640,17 @@
       <c r="I21" s="1">
         <v>19.920000000000002</v>
       </c>
+      <c r="R21" s="3">
+        <v>8.4</v>
+      </c>
+      <c r="S21" s="3">
+        <v>-21</v>
+      </c>
+      <c r="T21" s="3">
+        <v>195</v>
+      </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="4">
         <v>44245</v>
       </c>
@@ -3420,10 +3661,12 @@
         <v>37.36</v>
       </c>
       <c r="D22" s="3">
-        <v>-13</v>
+        <f t="shared" si="0"/>
+        <v>-20</v>
       </c>
       <c r="E22" s="3">
-        <v>196</v>
+        <f t="shared" si="1"/>
+        <v>123</v>
       </c>
       <c r="F22" s="1">
         <v>19.27</v>
@@ -3437,8 +3680,17 @@
       <c r="I22" s="1">
         <v>18.77</v>
       </c>
+      <c r="R22" s="3">
+        <v>37.36</v>
+      </c>
+      <c r="S22" s="3">
+        <v>-13</v>
+      </c>
+      <c r="T22" s="3">
+        <v>196</v>
+      </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="4">
         <v>44245</v>
       </c>
@@ -3449,10 +3701,12 @@
         <v>1.25</v>
       </c>
       <c r="D23" s="3">
-        <v>-25</v>
+        <f t="shared" si="0"/>
+        <v>-32</v>
       </c>
       <c r="E23" s="3">
-        <v>197</v>
+        <f t="shared" si="1"/>
+        <v>124</v>
       </c>
       <c r="F23">
         <v>21.007908152462601</v>
@@ -3465,6 +3719,54 @@
       </c>
       <c r="I23">
         <v>20.4612415214939</v>
+      </c>
+      <c r="R23" s="3">
+        <v>1.25</v>
+      </c>
+      <c r="S23" s="3">
+        <v>-25</v>
+      </c>
+      <c r="T23" s="3">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24" s="4">
+        <v>44260</v>
+      </c>
+      <c r="B24" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="C24" s="3">
+        <v>36.493385950724246</v>
+      </c>
+      <c r="D24" s="3">
+        <v>-18</v>
+      </c>
+      <c r="E24" s="3">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25" s="4">
+        <v>44260</v>
+      </c>
+      <c r="B25" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D25" s="3">
+        <f>D24-S15</f>
+        <v>-7</v>
+      </c>
+      <c r="E25" s="3">
+        <f>E24-T15</f>
+        <v>-73</v>
+      </c>
+      <c r="F25" s="6" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>